<commit_message>
update mcode to 0.9 candidate 1
</commit_message>
<xml_diff>
--- a/docs/mcode/oncocore-CancerStageTiming-extension.xlsx
+++ b/docs/mcode/oncocore-CancerStageTiming-extension.xlsx
@@ -204,7 +204,7 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/projectURL/oncocore/vs/CancerStageTimingVS</t>
+    <t>http://hl7.org/fhir/us/mcode/oncocore/vs/CancerStageTimingVS</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -389,7 +389,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="63.12890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="59.32421875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>

</xml_diff>